<commit_message>
Time cost functions working again
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Short_Solutions.xlsx
+++ b/data/TR/results/All_Short_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="13">
   <si>
     <t>Filename</t>
   </si>
@@ -169,126 +169,72 @@
         <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>32.0</v>
+        <v>44.0</v>
       </c>
       <c r="G8" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="U8" t="n">
         <v>34.0</v>
       </c>
-      <c r="H8" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>14.0</v>
-      </c>
       <c r="V8" t="n">
-        <v>17.0</v>
+        <v>4.0</v>
       </c>
       <c r="W8" t="n">
-        <v>33.0</v>
+        <v>5.0</v>
       </c>
       <c r="X8" t="n">
-        <v>31.0</v>
+        <v>40.0</v>
       </c>
       <c r="Y8" t="n">
-        <v>30.0</v>
+        <v>39.0</v>
       </c>
       <c r="Z8" t="n">
-        <v>36.0</v>
+        <v>6.0</v>
       </c>
       <c r="AA8" t="n">
-        <v>42.0</v>
+        <v>7.0</v>
       </c>
       <c r="AB8" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="AS8" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="AT8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -422,42 +368,24 @@
         <v>36.0</v>
       </c>
       <c r="P10" t="n">
-        <v>42.0</v>
+        <v>50.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>41.0</v>
+        <v>57.0</v>
       </c>
       <c r="R10" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="S10" t="n">
         <v>44.0</v>
       </c>
-      <c r="S10" t="n">
-        <v>45.0</v>
-      </c>
       <c r="T10" t="n">
-        <v>50.0</v>
+        <v>39.0</v>
       </c>
       <c r="U10" t="n">
-        <v>49.0</v>
+        <v>40.0</v>
       </c>
       <c r="V10" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="X10" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="AB10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -561,66 +489,48 @@
         <v>0.0</v>
       </c>
       <c r="F12" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="S12" t="n">
         <v>40.0</v>
       </c>
-      <c r="G12" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>26.0</v>
-      </c>
       <c r="T12" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="X12" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="Z12" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added classes for reading and writing with TR based on file input type -- will add support for PVRP file type in near future
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Short_Solutions.xlsx
+++ b/data/TR/results/All_Short_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Filename</t>
   </si>
@@ -23,13 +23,13 @@
     <t>Selection Type</t>
   </si>
   <si>
-    <t>edu.sru.thangiah.zeus.tr.TRSolutionHierarchy.Heuristics.Selection.TRClosestDistanceToDepot</t>
+    <t>TRClosestDistanceToDepot</t>
   </si>
   <si>
     <t>Insertion Type</t>
   </si>
   <si>
-    <t>edu.sru.thangiah.zeus.tr.TRSolutionHierarchy.Heuristics.Insertion.TRGreedyInsertion</t>
+    <t>TRGreedyInsertion</t>
   </si>
   <si>
     <t>Depot</t>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Nodes --&gt;</t>
-  </si>
-  <si>
-    <t>TRClosestDistanceToDepot</t>
-  </si>
-  <si>
-    <t>TRGreedyInsertion</t>
   </si>
 </sst>
 </file>
@@ -122,7 +116,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -130,7 +124,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5"/>

</xml_diff>

<commit_message>
PVRP format working. Few bugs need ironed out -- mostly that PVRP format is being scheduled multiple times (the nodes)
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Short_Solutions.xlsx
+++ b/data/TR/results/All_Short_Solutions.xlsx
@@ -6,18 +6,18 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="p14.xlsx" r:id="rId3" sheetId="1"/>
+    <sheet name="TrashRoutes-Frequency.xlsx" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Filename</t>
   </si>
   <si>
-    <t>p14.xlsx</t>
+    <t>TrashRoutes-Frequency.xlsx</t>
   </si>
   <si>
     <t>Selection Type</t>
@@ -157,72 +157,78 @@
         <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>44.0</v>
+        <v>108.0</v>
       </c>
       <c r="E8" t="n">
         <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>20.0</v>
+        <v>44.0</v>
       </c>
       <c r="G8" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="Q8" t="n">
         <v>19.0</v>
       </c>
-      <c r="H8" t="n">
+      <c r="R8" t="n">
         <v>18.0</v>
       </c>
-      <c r="I8" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="S8" t="n">
         <v>11.0</v>
       </c>
-      <c r="P8" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>7.0</v>
-      </c>
       <c r="T8" t="n">
-        <v>6.0</v>
+        <v>33.0</v>
       </c>
       <c r="U8" t="n">
-        <v>5.0</v>
+        <v>34.0</v>
       </c>
       <c r="V8" t="n">
         <v>4.0</v>
       </c>
       <c r="W8" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="X8" t="n">
-        <v>2.0</v>
+        <v>40.0</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.0</v>
+        <v>39.0</v>
       </c>
       <c r="Z8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="AB8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -237,12 +243,75 @@
         <v>1.0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>124.0</v>
       </c>
       <c r="E9" t="n">
         <v>0.0</v>
       </c>
       <c r="F9" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="AA9" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -257,12 +326,60 @@
         <v>2.0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>97.0</v>
       </c>
       <c r="E10" t="n">
         <v>0.0</v>
       </c>
       <c r="F10" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="V10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -277,12 +394,75 @@
         <v>3.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>124.0</v>
       </c>
       <c r="E11" t="n">
         <v>0.0</v>
       </c>
       <c r="F11" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="AA11" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -294,75 +474,57 @@
         <v>-1.0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D12" t="n">
-        <v>44.0</v>
+        <v>92.0</v>
       </c>
       <c r="E12" t="n">
         <v>0.0</v>
       </c>
       <c r="F12" t="n">
-        <v>20.0</v>
+        <v>36.0</v>
       </c>
       <c r="G12" t="n">
-        <v>19.0</v>
+        <v>34.0</v>
       </c>
       <c r="H12" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="I12" t="n">
         <v>18.0</v>
       </c>
-      <c r="I12" t="n">
-        <v>17.0</v>
-      </c>
       <c r="J12" t="n">
-        <v>16.0</v>
+        <v>26.0</v>
       </c>
       <c r="K12" t="n">
-        <v>15.0</v>
+        <v>27.0</v>
       </c>
       <c r="L12" t="n">
-        <v>14.0</v>
+        <v>29.0</v>
       </c>
       <c r="M12" t="n">
-        <v>13.0</v>
+        <v>28.0</v>
       </c>
       <c r="N12" t="n">
-        <v>12.0</v>
+        <v>30.0</v>
       </c>
       <c r="O12" t="n">
-        <v>11.0</v>
+        <v>50.0</v>
       </c>
       <c r="P12" t="n">
-        <v>10.0</v>
+        <v>57.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>9.0</v>
+        <v>49.0</v>
       </c>
       <c r="R12" t="n">
-        <v>8.0</v>
+        <v>44.0</v>
       </c>
       <c r="S12" t="n">
-        <v>7.0</v>
+        <v>40.0</v>
       </c>
       <c r="T12" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="X12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="Z12" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -374,55 +536,69 @@
         <v>-1.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="E13" t="n">
         <v>0.0</v>
       </c>
       <c r="F13" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="B14" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="B15" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="X13" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generic compositions finished and working
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Short_Solutions.xlsx
+++ b/data/TR/results/All_Short_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="11">
   <si>
     <t>Filename</t>
   </si>
@@ -157,78 +157,132 @@
         <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>108.0</v>
+        <v>150.0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="AJ8" t="n">
         <v>44.0</v>
       </c>
-      <c r="G8" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="V8" t="n">
+      <c r="AK8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AS8" t="n">
         <v>4.0</v>
       </c>
-      <c r="W8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="AB8" t="n">
+      <c r="AT8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -246,7 +300,7 @@
         <v>124.0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F9" t="n">
         <v>46.0</v>
@@ -326,10 +380,10 @@
         <v>2.0</v>
       </c>
       <c r="D10" t="n">
-        <v>97.0</v>
+        <v>121.0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F10" t="n">
         <v>34.0</v>
@@ -362,24 +416,42 @@
         <v>36.0</v>
       </c>
       <c r="P10" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="T10" t="n">
         <v>50.0</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="U10" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="V10" t="n">
         <v>57.0</v>
       </c>
-      <c r="R10" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="T10" t="n">
+      <c r="W10" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="Z10" t="n">
         <v>39.0</v>
       </c>
-      <c r="U10" t="n">
+      <c r="AA10" t="n">
         <v>40.0</v>
       </c>
-      <c r="V10" t="n">
+      <c r="AB10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -397,7 +469,7 @@
         <v>124.0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F11" t="n">
         <v>46.0</v>
@@ -477,54 +549,72 @@
         <v>4.0</v>
       </c>
       <c r="D12" t="n">
-        <v>92.0</v>
+        <v>116.0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F12" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="W12" t="n">
         <v>36.0</v>
       </c>
-      <c r="G12" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="T12" t="n">
+      <c r="X12" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="Z12" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -542,7 +632,7 @@
         <v>103.0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="F13" t="n">
         <v>36.0</v>

</xml_diff>

<commit_message>
Full PVRP and TR support. Scheduling issue fixed.
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Short_Solutions.xlsx
+++ b/data/TR/results/All_Short_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
   <si>
     <t>Filename</t>
   </si>
@@ -157,132 +157,66 @@
         <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>150.0</v>
+        <v>103.0</v>
       </c>
       <c r="E8" t="n">
         <v>-1.0</v>
       </c>
       <c r="F8" t="n">
-        <v>9.0</v>
+        <v>36.0</v>
       </c>
       <c r="G8" t="n">
         <v>34.0</v>
       </c>
       <c r="H8" t="n">
-        <v>13.0</v>
+        <v>31.0</v>
       </c>
       <c r="I8" t="n">
-        <v>11.0</v>
+        <v>33.0</v>
       </c>
       <c r="J8" t="n">
-        <v>12.0</v>
+        <v>18.0</v>
       </c>
       <c r="K8" t="n">
-        <v>16.0</v>
+        <v>25.0</v>
       </c>
       <c r="L8" t="n">
-        <v>19.0</v>
+        <v>22.0</v>
       </c>
       <c r="M8" t="n">
-        <v>20.0</v>
+        <v>26.0</v>
       </c>
       <c r="N8" t="n">
-        <v>21.0</v>
+        <v>27.0</v>
       </c>
       <c r="O8" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="P8" t="n">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>28.0</v>
+        <v>30.0</v>
       </c>
       <c r="R8" t="n">
-        <v>27.0</v>
+        <v>38.0</v>
       </c>
       <c r="S8" t="n">
-        <v>18.0</v>
+        <v>57.0</v>
       </c>
       <c r="T8" t="n">
-        <v>15.0</v>
+        <v>49.0</v>
       </c>
       <c r="U8" t="n">
-        <v>14.0</v>
+        <v>44.0</v>
       </c>
       <c r="V8" t="n">
-        <v>17.0</v>
+        <v>39.0</v>
       </c>
       <c r="W8" t="n">
-        <v>33.0</v>
+        <v>40.0</v>
       </c>
       <c r="X8" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>45.0</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="AS8" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="AT8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -297,75 +231,132 @@
         <v>1.0</v>
       </c>
       <c r="D9" t="n">
-        <v>124.0</v>
+        <v>150.0</v>
       </c>
       <c r="E9" t="n">
         <v>-1.0</v>
       </c>
       <c r="F9" t="n">
-        <v>46.0</v>
+        <v>9.0</v>
       </c>
       <c r="G9" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="AE9" t="n">
         <v>49.0</v>
       </c>
-      <c r="H9" t="n">
-        <v>51.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="AF9" t="n">
         <v>57.0</v>
       </c>
-      <c r="L9" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>52.0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="S9" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="U9" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="AA9" t="n">
+      <c r="AG9" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="AT9" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -380,78 +371,75 @@
         <v>2.0</v>
       </c>
       <c r="D10" t="n">
-        <v>121.0</v>
+        <v>124.0</v>
       </c>
       <c r="E10" t="n">
         <v>-1.0</v>
       </c>
       <c r="F10" t="n">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="G10" t="n">
-        <v>39.0</v>
+        <v>49.0</v>
       </c>
       <c r="H10" t="n">
-        <v>47.0</v>
+        <v>51.0</v>
       </c>
       <c r="I10" t="n">
-        <v>48.0</v>
+        <v>50.0</v>
       </c>
       <c r="J10" t="n">
-        <v>59.0</v>
+        <v>58.0</v>
       </c>
       <c r="K10" t="n">
         <v>57.0</v>
       </c>
       <c r="L10" t="n">
-        <v>49.0</v>
+        <v>56.0</v>
       </c>
       <c r="M10" t="n">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
       <c r="N10" t="n">
-        <v>45.0</v>
+        <v>53.0</v>
       </c>
       <c r="O10" t="n">
-        <v>44.0</v>
+        <v>37.0</v>
       </c>
       <c r="P10" t="n">
-        <v>41.0</v>
+        <v>38.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>42.0</v>
+        <v>30.0</v>
       </c>
       <c r="R10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="Y10" t="n">
         <v>36.0</v>
       </c>
-      <c r="S10" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="T10" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="U10" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="X10" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>18.0</v>
-      </c>
       <c r="Z10" t="n">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
       <c r="AA10" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="AB10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -466,75 +454,78 @@
         <v>3.0</v>
       </c>
       <c r="D11" t="n">
-        <v>124.0</v>
+        <v>121.0</v>
       </c>
       <c r="E11" t="n">
         <v>-1.0</v>
       </c>
       <c r="F11" t="n">
-        <v>46.0</v>
+        <v>40.0</v>
       </c>
       <c r="G11" t="n">
-        <v>49.0</v>
+        <v>39.0</v>
       </c>
       <c r="H11" t="n">
-        <v>51.0</v>
+        <v>47.0</v>
       </c>
       <c r="I11" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
       </c>
       <c r="J11" t="n">
-        <v>58.0</v>
+        <v>59.0</v>
       </c>
       <c r="K11" t="n">
         <v>57.0</v>
       </c>
       <c r="L11" t="n">
-        <v>56.0</v>
+        <v>49.0</v>
       </c>
       <c r="M11" t="n">
-        <v>52.0</v>
+        <v>50.0</v>
       </c>
       <c r="N11" t="n">
-        <v>53.0</v>
+        <v>45.0</v>
       </c>
       <c r="O11" t="n">
-        <v>37.0</v>
+        <v>44.0</v>
       </c>
       <c r="P11" t="n">
-        <v>38.0</v>
+        <v>41.0</v>
       </c>
       <c r="Q11" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="T11" t="n">
         <v>30.0</v>
       </c>
-      <c r="R11" t="n">
+      <c r="U11" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="Y11" t="n">
         <v>18.0</v>
       </c>
-      <c r="S11" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="U11" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="X11" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>36.0</v>
-      </c>
       <c r="Z11" t="n">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
       <c r="AA11" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="AB11" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -549,72 +540,75 @@
         <v>4.0</v>
       </c>
       <c r="D12" t="n">
-        <v>116.0</v>
+        <v>124.0</v>
       </c>
       <c r="E12" t="n">
         <v>-1.0</v>
       </c>
       <c r="F12" t="n">
-        <v>40.0</v>
+        <v>46.0</v>
       </c>
       <c r="G12" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="H12" t="n">
-        <v>48.0</v>
+        <v>51.0</v>
       </c>
       <c r="I12" t="n">
-        <v>59.0</v>
+        <v>50.0</v>
       </c>
       <c r="J12" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="K12" t="n">
         <v>57.0</v>
       </c>
-      <c r="K12" t="n">
-        <v>50.0</v>
-      </c>
       <c r="L12" t="n">
-        <v>49.0</v>
+        <v>56.0</v>
       </c>
       <c r="M12" t="n">
-        <v>44.0</v>
+        <v>52.0</v>
       </c>
       <c r="N12" t="n">
-        <v>45.0</v>
+        <v>53.0</v>
       </c>
       <c r="O12" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="Q12" t="n">
         <v>30.0</v>
       </c>
-      <c r="P12" t="n">
+      <c r="R12" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="X12" t="n">
         <v>28.0</v>
       </c>
-      <c r="Q12" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="W12" t="n">
+      <c r="Y12" t="n">
         <v>36.0</v>
       </c>
-      <c r="X12" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>41.0</v>
-      </c>
       <c r="Z12" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="AA12" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -629,66 +623,72 @@
         <v>5.0</v>
       </c>
       <c r="D13" t="n">
-        <v>103.0</v>
+        <v>116.0</v>
       </c>
       <c r="E13" t="n">
         <v>-1.0</v>
       </c>
       <c r="F13" t="n">
-        <v>36.0</v>
+        <v>40.0</v>
       </c>
       <c r="G13" t="n">
-        <v>34.0</v>
+        <v>47.0</v>
       </c>
       <c r="H13" t="n">
-        <v>31.0</v>
+        <v>48.0</v>
       </c>
       <c r="I13" t="n">
-        <v>33.0</v>
+        <v>59.0</v>
       </c>
       <c r="J13" t="n">
-        <v>18.0</v>
+        <v>57.0</v>
       </c>
       <c r="K13" t="n">
-        <v>25.0</v>
+        <v>50.0</v>
       </c>
       <c r="L13" t="n">
-        <v>22.0</v>
+        <v>49.0</v>
       </c>
       <c r="M13" t="n">
-        <v>26.0</v>
+        <v>44.0</v>
       </c>
       <c r="N13" t="n">
-        <v>27.0</v>
+        <v>45.0</v>
       </c>
       <c r="O13" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="P13" t="n">
         <v>28.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
       <c r="R13" t="n">
-        <v>38.0</v>
+        <v>27.0</v>
       </c>
       <c r="S13" t="n">
-        <v>57.0</v>
+        <v>26.0</v>
       </c>
       <c r="T13" t="n">
-        <v>49.0</v>
+        <v>18.0</v>
       </c>
       <c r="U13" t="n">
-        <v>44.0</v>
+        <v>31.0</v>
       </c>
       <c r="V13" t="n">
-        <v>39.0</v>
+        <v>34.0</v>
       </c>
       <c r="W13" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="X13" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="Z13" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
selection update and weighted insertion in the works
</commit_message>
<xml_diff>
--- a/data/TR/results/All_Short_Solutions.xlsx
+++ b/data/TR/results/All_Short_Solutions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Filename</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Selection Type</t>
   </si>
   <si>
-    <t>TRClosestDistanceToDepot</t>
+    <t>TRChooseByHighestDemand</t>
   </si>
   <si>
     <t>Insertion Type</t>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Nodes --&gt;</t>
-  </si>
-  <si>
-    <t>TRSmallestAngleClosestDistanceToDepot</t>
-  </si>
-  <si>
-    <t>TRSmallestAngleToDepot</t>
   </si>
 </sst>
 </file>
@@ -122,7 +116,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -163,72 +157,69 @@
         <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>109.0</v>
+        <v>108.0</v>
       </c>
       <c r="E8" t="n">
         <v>-1.0</v>
       </c>
       <c r="F8" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="G8" t="n">
         <v>38.0</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>36.0</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>34.0</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>31.0</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>30.0</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>18.0</v>
       </c>
-      <c r="L8" t="n">
-        <v>22.0</v>
-      </c>
       <c r="M8" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="N8" t="n">
         <v>26.0</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>27.0</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>29.0</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>28.0</v>
       </c>
-      <c r="Q8" t="n">
-        <v>52.0</v>
-      </c>
       <c r="R8" t="n">
-        <v>56.0</v>
+        <v>57.0</v>
       </c>
       <c r="S8" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="T8" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="U8" t="n">
-        <v>49.0</v>
+        <v>44.0</v>
       </c>
       <c r="V8" t="n">
-        <v>44.0</v>
+        <v>46.0</v>
       </c>
       <c r="W8" t="n">
-        <v>46.0</v>
+        <v>39.0</v>
       </c>
       <c r="X8" t="n">
-        <v>39.0</v>
+        <v>40.0</v>
       </c>
       <c r="Y8" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -243,63 +234,69 @@
         <v>1.0</v>
       </c>
       <c r="D9" t="n">
-        <v>102.0</v>
+        <v>108.0</v>
       </c>
       <c r="E9" t="n">
         <v>-1.0</v>
       </c>
       <c r="F9" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="G9" t="n">
-        <v>58.0</v>
+        <v>34.0</v>
       </c>
       <c r="H9" t="n">
-        <v>57.0</v>
+        <v>33.0</v>
       </c>
       <c r="I9" t="n">
-        <v>49.0</v>
+        <v>31.0</v>
       </c>
       <c r="J9" t="n">
-        <v>51.0</v>
+        <v>30.0</v>
       </c>
       <c r="K9" t="n">
-        <v>53.0</v>
+        <v>18.0</v>
       </c>
       <c r="L9" t="n">
-        <v>30.0</v>
+        <v>19.0</v>
       </c>
       <c r="M9" t="n">
-        <v>28.0</v>
+        <v>22.0</v>
       </c>
       <c r="N9" t="n">
-        <v>29.0</v>
+        <v>26.0</v>
       </c>
       <c r="O9" t="n">
         <v>27.0</v>
       </c>
       <c r="P9" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="R9" t="n">
-        <v>18.0</v>
+        <v>53.0</v>
       </c>
       <c r="S9" t="n">
-        <v>11.0</v>
+        <v>50.0</v>
       </c>
       <c r="T9" t="n">
-        <v>33.0</v>
+        <v>57.0</v>
       </c>
       <c r="U9" t="n">
-        <v>31.0</v>
+        <v>49.0</v>
       </c>
       <c r="V9" t="n">
-        <v>36.0</v>
+        <v>44.0</v>
       </c>
       <c r="W9" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="Y9" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -314,75 +311,66 @@
         <v>2.0</v>
       </c>
       <c r="D10" t="n">
-        <v>110.0</v>
+        <v>108.0</v>
       </c>
       <c r="E10" t="n">
         <v>-1.0</v>
       </c>
       <c r="F10" t="n">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="G10" t="n">
-        <v>36.0</v>
+        <v>31.0</v>
       </c>
       <c r="H10" t="n">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="I10" t="n">
-        <v>34.0</v>
+        <v>11.0</v>
       </c>
       <c r="J10" t="n">
-        <v>33.0</v>
+        <v>18.0</v>
       </c>
       <c r="K10" t="n">
-        <v>18.0</v>
+        <v>25.0</v>
       </c>
       <c r="L10" t="n">
-        <v>19.0</v>
+        <v>26.0</v>
       </c>
       <c r="M10" t="n">
-        <v>22.0</v>
+        <v>27.0</v>
       </c>
       <c r="N10" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="O10" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="P10" t="n">
-        <v>29.0</v>
+        <v>38.0</v>
       </c>
       <c r="Q10" t="n">
-        <v>28.0</v>
+        <v>56.0</v>
       </c>
       <c r="R10" t="n">
-        <v>30.0</v>
+        <v>57.0</v>
       </c>
       <c r="S10" t="n">
-        <v>38.0</v>
+        <v>50.0</v>
       </c>
       <c r="T10" t="n">
-        <v>52.0</v>
+        <v>49.0</v>
       </c>
       <c r="U10" t="n">
-        <v>56.0</v>
+        <v>44.0</v>
       </c>
       <c r="V10" t="n">
-        <v>57.0</v>
+        <v>46.0</v>
       </c>
       <c r="W10" t="n">
-        <v>50.0</v>
+        <v>5.0</v>
       </c>
       <c r="X10" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="AA10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -397,7 +385,7 @@
         <v>3.0</v>
       </c>
       <c r="D11" t="n">
-        <v>109.0</v>
+        <v>108.0</v>
       </c>
       <c r="E11" t="n">
         <v>-1.0</v>
@@ -412,51 +400,54 @@
         <v>34.0</v>
       </c>
       <c r="I11" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="J11" t="n">
         <v>18.0</v>
       </c>
-      <c r="J11" t="n">
-        <v>25.0</v>
-      </c>
       <c r="K11" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="L11" t="n">
         <v>26.0</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>27.0</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>29.0</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>28.0</v>
       </c>
-      <c r="O11" t="n">
-        <v>30.0</v>
-      </c>
       <c r="P11" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="Q11" t="n">
         <v>51.0</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>50.0</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>57.0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>58.0</v>
       </c>
       <c r="T11" t="n">
         <v>49.0</v>
       </c>
       <c r="U11" t="n">
-        <v>44.0</v>
+        <v>39.0</v>
       </c>
       <c r="V11" t="n">
         <v>40.0</v>
       </c>
       <c r="W11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="X11" t="n">
         <v>4.0</v>
       </c>
-      <c r="X11" t="n">
+      <c r="Y11" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -471,72 +462,66 @@
         <v>4.0</v>
       </c>
       <c r="D12" t="n">
-        <v>109.0</v>
+        <v>108.0</v>
       </c>
       <c r="E12" t="n">
         <v>-1.0</v>
       </c>
       <c r="F12" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="H12" t="n">
         <v>36.0</v>
       </c>
-      <c r="G12" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>31.0</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="K12" t="n">
         <v>33.0</v>
       </c>
-      <c r="J12" t="n">
+      <c r="L12" t="n">
         <v>18.0</v>
       </c>
-      <c r="K12" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="N12" t="n">
         <v>26.0</v>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>27.0</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>29.0</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
         <v>28.0</v>
       </c>
-      <c r="P12" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>38.0</v>
-      </c>
       <c r="R12" t="n">
-        <v>37.0</v>
+        <v>56.0</v>
       </c>
       <c r="S12" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="U12" t="n">
         <v>50.0</v>
       </c>
-      <c r="T12" t="n">
-        <v>57.0</v>
-      </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>49.0</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>44.0</v>
       </c>
-      <c r="W12" t="n">
-        <v>46.0</v>
-      </c>
       <c r="X12" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="Z12" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -551,7 +536,7 @@
         <v>5.0</v>
       </c>
       <c r="D13" t="n">
-        <v>109.0</v>
+        <v>108.0</v>
       </c>
       <c r="E13" t="n">
         <v>-1.0</v>
@@ -563,48 +548,57 @@
         <v>36.0</v>
       </c>
       <c r="H13" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="J13" t="n">
         <v>30.0</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="n">
         <v>18.0</v>
       </c>
-      <c r="J13" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="M13" t="n">
         <v>26.0</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>27.0</v>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>29.0</v>
       </c>
-      <c r="N13" t="n">
+      <c r="P13" t="n">
         <v>28.0</v>
       </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
         <v>53.0</v>
       </c>
-      <c r="P13" t="n">
+      <c r="R13" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="T13" t="n">
         <v>50.0</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="U13" t="n">
         <v>57.0</v>
       </c>
-      <c r="R13" t="n">
+      <c r="V13" t="n">
         <v>49.0</v>
       </c>
-      <c r="S13" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="T13" t="n">
+      <c r="W13" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="X13" t="n">
         <v>40.0</v>
       </c>
-      <c r="U13" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="V13" t="n">
+      <c r="Y13" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>